<commit_message>
Sometimes I hate you GP
Finished SM graphs
</commit_message>
<xml_diff>
--- a/Data/ChannelDescription.xlsx
+++ b/Data/ChannelDescription.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LinaBarbosa/Documents/GitHub/Model/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lina/Documents/GitHub/Model/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="460" windowWidth="25600" windowHeight="14220" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="7040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="91">
   <si>
     <t>X</t>
   </si>
@@ -137,27 +140,15 @@
     <t>grass</t>
   </si>
   <si>
-    <t>Silt to Fine sand</t>
-  </si>
-  <si>
-    <t>Coarse gravel with sand</t>
-  </si>
-  <si>
     <t xml:space="preserve">ragweed </t>
   </si>
   <si>
-    <t xml:space="preserve">Silt-medium sand </t>
-  </si>
-  <si>
     <t>bedrock sycamore tree</t>
   </si>
   <si>
     <t>20-35</t>
   </si>
   <si>
-    <t>coarse to very course sand</t>
-  </si>
-  <si>
     <t>bare ground</t>
   </si>
   <si>
@@ -167,9 +158,6 @@
     <t>silt coarse sand over bedrock</t>
   </si>
   <si>
-    <t>silt very coarse sand</t>
-  </si>
-  <si>
     <t>Bay laurel, grasses all over</t>
   </si>
   <si>
@@ -182,9 +170,6 @@
     <t>bull rock over bedrock</t>
   </si>
   <si>
-    <t>BEdrock</t>
-  </si>
-  <si>
     <t>bare, tree rooted oak</t>
   </si>
   <si>
@@ -197,9 +182,6 @@
     <t>Projection of bank from upstream</t>
   </si>
   <si>
-    <t>Medium sand</t>
-  </si>
-  <si>
     <t>gravel over bed rock</t>
   </si>
   <si>
@@ -224,21 +206,12 @@
     <t>brushes</t>
   </si>
   <si>
-    <t xml:space="preserve">Medium sand and silt </t>
-  </si>
-  <si>
     <t>grass and shurbs</t>
   </si>
   <si>
     <t xml:space="preserve">ragweed, sparse grass </t>
   </si>
   <si>
-    <t>very fine sand</t>
-  </si>
-  <si>
-    <t>sandy silt</t>
-  </si>
-  <si>
     <t>grass, mulefat</t>
   </si>
   <si>
@@ -248,18 +221,12 @@
     <t>Bedrock, Oak tree in the riparian zone</t>
   </si>
   <si>
-    <t>fine to mid sand</t>
-  </si>
-  <si>
     <t>grass, ragweed and sycamore</t>
   </si>
   <si>
     <t>coarse sand over bedrock</t>
   </si>
   <si>
-    <t xml:space="preserve">coarse sand </t>
-  </si>
-  <si>
     <t>30-35</t>
   </si>
   <si>
@@ -272,9 +239,6 @@
     <t>seeps</t>
   </si>
   <si>
-    <t>Moist cover rich silt very fine sand</t>
-  </si>
-  <si>
     <t>cat tails, wild cucumber brushes</t>
   </si>
   <si>
@@ -309,6 +273,33 @@
   </si>
   <si>
     <t>Depth</t>
+  </si>
+  <si>
+    <t>Coarse sand</t>
+  </si>
+  <si>
+    <t>sand</t>
+  </si>
+  <si>
+    <t>silt-clay loam</t>
+  </si>
+  <si>
+    <t>silt loam</t>
+  </si>
+  <si>
+    <t>Silty loam</t>
+  </si>
+  <si>
+    <t>silty loam</t>
+  </si>
+  <si>
+    <t>Moist cover rich silty loam</t>
+  </si>
+  <si>
+    <t>Coarse gravel</t>
+  </si>
+  <si>
+    <t>Very fine sand</t>
   </si>
 </sst>
 </file>
@@ -636,8 +627,8 @@
   <dimension ref="A1:T106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H95" sqref="H95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -660,24 +651,24 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="D1" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="E1" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>30</v>
@@ -707,7 +698,7 @@
         <v>7</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -947,7 +938,7 @@
         <v>9</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>24</v>
+        <v>89</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>9</v>
@@ -1075,7 +1066,7 @@
         <v>9</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>28</v>
@@ -1107,7 +1098,7 @@
         <v>9</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>29</v>
@@ -1235,7 +1226,7 @@
         <v>9</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>32</v>
@@ -1267,7 +1258,7 @@
         <v>9</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>32</v>
@@ -1395,7 +1386,7 @@
         <v>9</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>34</v>
@@ -1427,7 +1418,7 @@
         <v>9</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>36</v>
@@ -1523,10 +1514,10 @@
         <v>9</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J27" s="1">
         <v>2212</v>
@@ -1587,10 +1578,10 @@
         <v>9</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J29" s="1">
         <v>218</v>
@@ -1677,16 +1668,16 @@
         <v>9</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J32" s="1">
         <v>218</v>
@@ -1712,7 +1703,7 @@
         <v>9</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>23</v>
@@ -1747,10 +1738,10 @@
         <v>9</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J34" s="1">
         <v>2225</v>
@@ -1843,10 +1834,10 @@
         <v>9</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="J37" s="1">
         <v>2225</v>
@@ -1875,10 +1866,10 @@
         <v>9</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J38" s="1">
         <v>2231</v>
@@ -1910,7 +1901,7 @@
         <v>24</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J39" s="1">
         <v>2231</v>
@@ -2006,7 +1997,7 @@
         <v>24</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J42" s="1">
         <v>2231</v>
@@ -2035,7 +2026,7 @@
         <v>9</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>36</v>
@@ -2067,10 +2058,10 @@
         <v>9</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J44" s="1">
         <v>2236</v>
@@ -2157,16 +2148,16 @@
         <v>9</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J47" s="1">
         <v>2236</v>
@@ -2195,7 +2186,7 @@
         <v>9</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>9</v>
@@ -2204,7 +2195,7 @@
         <v>2241</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
@@ -2233,7 +2224,7 @@
         <v>9</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>9</v>
@@ -2329,7 +2320,7 @@
         <v>9</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>9</v>
@@ -2361,7 +2352,7 @@
         <v>9</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>36</v>
@@ -2393,7 +2384,7 @@
         <v>9</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>36</v>
@@ -2483,13 +2474,13 @@
         <v>9</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>36</v>
@@ -2521,7 +2512,7 @@
         <v>9</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>9</v>
@@ -2553,7 +2544,7 @@
         <v>9</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>9</v>
@@ -2649,7 +2640,7 @@
         <v>9</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>9</v>
@@ -2707,16 +2698,16 @@
         <v>0</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="J64" s="1">
         <v>2255</v>
@@ -2803,16 +2794,16 @@
         <v>9</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J67" s="1">
         <v>2255</v>
@@ -2841,10 +2832,10 @@
         <v>9</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="J68" s="1">
         <v>2259</v>
@@ -2873,10 +2864,10 @@
         <v>9</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="J69" s="1">
         <v>2259</v>
@@ -2969,10 +2960,10 @@
         <v>9</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="J72" s="1">
         <v>2259</v>
@@ -3001,7 +2992,7 @@
         <v>9</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>36</v>
@@ -3033,7 +3024,7 @@
         <v>9</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>36</v>
@@ -3106,7 +3097,7 @@
         <v>2264</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
@@ -3132,7 +3123,7 @@
         <v>9</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="I77" s="1" t="s">
         <v>25</v>
@@ -3141,7 +3132,7 @@
         <v>2264</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
@@ -3167,10 +3158,10 @@
         <v>9</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J78" s="1">
         <v>2268</v>
@@ -3199,10 +3190,10 @@
         <v>9</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="J79" s="1">
         <v>2268</v>
@@ -3295,16 +3286,16 @@
         <v>9</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J82" s="1">
         <v>2268</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
@@ -3330,7 +3321,7 @@
         <v>9</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="I83" s="1" t="s">
         <v>36</v>
@@ -3339,7 +3330,7 @@
         <v>2274</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
@@ -3493,10 +3484,10 @@
         <v>9</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="J88" s="1">
         <v>2279</v>
@@ -3525,7 +3516,7 @@
         <v>9</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="I89" s="1" t="s">
         <v>36</v>
@@ -3621,10 +3612,10 @@
         <v>9</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="J92" s="1">
         <v>2279</v>
@@ -3653,16 +3644,16 @@
         <v>9</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="J93" s="1">
         <v>2285</v>
       </c>
       <c r="K93" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
@@ -3682,22 +3673,22 @@
         <v>0</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="J94" s="1">
         <v>2285</v>
       </c>
       <c r="K94" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
@@ -3732,7 +3723,7 @@
         <v>2285</v>
       </c>
       <c r="K95" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
@@ -3767,7 +3758,7 @@
         <v>2285</v>
       </c>
       <c r="K96" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
@@ -3793,16 +3784,16 @@
         <v>9</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J97" s="1">
         <v>2285</v>
       </c>
       <c r="K97" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
@@ -3828,16 +3819,16 @@
         <v>9</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="J98" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K98" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
@@ -3866,7 +3857,7 @@
         <v>24</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="J99" s="1" t="s">
         <v>9</v>
@@ -3959,10 +3950,10 @@
         <v>9</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="J102" s="1" t="s">
         <v>9</v>

</xml_diff>